<commit_message>
working and tested multiplication, reg r10 works correctly
</commit_message>
<xml_diff>
--- a/programing_models/Pixel_Flow.xlsx
+++ b/programing_models/Pixel_Flow.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ALL_Design" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Module_1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="80">
   <si>
     <t>name/tick</t>
   </si>
@@ -750,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN155"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
@@ -20118,8 +20118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39242,12 +39242,1935 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:41">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <f t="shared" ref="D1:I1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K1" s="1">
+        <f>J1+1</f>
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <f t="shared" ref="L1" si="1">K1+1</f>
+        <v>2</v>
+      </c>
+      <c r="M1" s="1">
+        <f t="shared" ref="M1" si="2">L1+1</f>
+        <v>3</v>
+      </c>
+      <c r="N1" s="1">
+        <f t="shared" ref="N1" si="3">M1+1</f>
+        <v>4</v>
+      </c>
+      <c r="O1" s="1">
+        <f t="shared" ref="O1" si="4">N1+1</f>
+        <v>5</v>
+      </c>
+      <c r="P1" s="1">
+        <f t="shared" ref="P1" si="5">O1+1</f>
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1">
+        <f t="shared" ref="Q1" si="6">P1+1</f>
+        <v>7</v>
+      </c>
+      <c r="R1" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="S1" s="1">
+        <f>R1+1</f>
+        <v>1</v>
+      </c>
+      <c r="T1" s="1">
+        <f t="shared" ref="T1" si="7">S1+1</f>
+        <v>2</v>
+      </c>
+      <c r="U1" s="1">
+        <f t="shared" ref="U1" si="8">T1+1</f>
+        <v>3</v>
+      </c>
+      <c r="V1" s="1">
+        <f t="shared" ref="V1" si="9">U1+1</f>
+        <v>4</v>
+      </c>
+      <c r="W1" s="1">
+        <f t="shared" ref="W1" si="10">V1+1</f>
+        <v>5</v>
+      </c>
+      <c r="X1" s="1">
+        <f t="shared" ref="X1" si="11">W1+1</f>
+        <v>6</v>
+      </c>
+      <c r="Y1" s="1">
+        <f t="shared" ref="Y1" si="12">X1+1</f>
+        <v>7</v>
+      </c>
+      <c r="Z1" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1">
+        <f>Z1+1</f>
+        <v>1</v>
+      </c>
+      <c r="AB1" s="1">
+        <f t="shared" ref="AB1" si="13">AA1+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC1" s="1">
+        <f t="shared" ref="AC1" si="14">AB1+1</f>
+        <v>3</v>
+      </c>
+      <c r="AD1" s="1">
+        <f t="shared" ref="AD1" si="15">AC1+1</f>
+        <v>4</v>
+      </c>
+      <c r="AE1" s="1">
+        <f t="shared" ref="AE1" si="16">AD1+1</f>
+        <v>5</v>
+      </c>
+      <c r="AF1" s="1">
+        <f t="shared" ref="AF1" si="17">AE1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AG1" s="1">
+        <f t="shared" ref="AG1" si="18">AF1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AH1" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AI1" s="1">
+        <f>AH1+1</f>
+        <v>1</v>
+      </c>
+      <c r="AJ1" s="1">
+        <f t="shared" ref="AJ1" si="19">AI1+1</f>
+        <v>2</v>
+      </c>
+      <c r="AK1" s="1">
+        <f t="shared" ref="AK1" si="20">AJ1+1</f>
+        <v>3</v>
+      </c>
+      <c r="AL1" s="1">
+        <f t="shared" ref="AL1" si="21">AK1+1</f>
+        <v>4</v>
+      </c>
+      <c r="AM1" s="1">
+        <f t="shared" ref="AM1" si="22">AL1+1</f>
+        <v>5</v>
+      </c>
+      <c r="AN1" s="1">
+        <f t="shared" ref="AN1" si="23">AM1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AO1" s="1">
+        <f t="shared" ref="AO1" si="24">AN1+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <f>B2</f>
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:P2" si="25">C2</f>
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="25"/>
+        <v>150</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="25"/>
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="25"/>
+        <v>150</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="25"/>
+        <v>100</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="25"/>
+        <v>150</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="25"/>
+        <v>100</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="25"/>
+        <v>150</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="26">N2</f>
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="27">O2</f>
+        <v>100</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ref="S2" si="28">P2</f>
+        <v>150</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ref="T2" si="29">Q2</f>
+        <v>10</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2" si="30">R2</f>
+        <v>100</v>
+      </c>
+      <c r="V2">
+        <f t="shared" ref="V2" si="31">S2</f>
+        <v>150</v>
+      </c>
+      <c r="W2">
+        <f t="shared" ref="W2" si="32">T2</f>
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <f t="shared" ref="X2" si="33">U2</f>
+        <v>100</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" ref="Y2" si="34">V2</f>
+        <v>150</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" ref="Z2:AA2" si="35">W2</f>
+        <v>10</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" ref="AB2" si="36">Y2</f>
+        <v>150</v>
+      </c>
+      <c r="AC2">
+        <f t="shared" ref="AC2" si="37">Z2</f>
+        <v>10</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" ref="AD2" si="38">AA2</f>
+        <v>100</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" ref="AE2" si="39">AB2</f>
+        <v>150</v>
+      </c>
+      <c r="AF2">
+        <f t="shared" ref="AF2" si="40">AC2</f>
+        <v>10</v>
+      </c>
+      <c r="AG2">
+        <f t="shared" ref="AG2" si="41">AD2</f>
+        <v>100</v>
+      </c>
+      <c r="AH2">
+        <f t="shared" ref="AH2" si="42">AE2</f>
+        <v>150</v>
+      </c>
+      <c r="AI2">
+        <f t="shared" ref="AI2" si="43">AF2</f>
+        <v>10</v>
+      </c>
+      <c r="AJ2">
+        <f t="shared" ref="AJ2" si="44">AG2</f>
+        <v>100</v>
+      </c>
+      <c r="AK2">
+        <f t="shared" ref="AK2:AL2" si="45">AH2</f>
+        <v>150</v>
+      </c>
+      <c r="AL2">
+        <f t="shared" si="45"/>
+        <v>10</v>
+      </c>
+      <c r="AM2">
+        <f t="shared" ref="AM2" si="46">AJ2</f>
+        <v>100</v>
+      </c>
+      <c r="AN2">
+        <f t="shared" ref="AN2" si="47">AK2</f>
+        <v>150</v>
+      </c>
+      <c r="AO2">
+        <f t="shared" ref="AO2" si="48">AL2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <f>B2+D2</f>
+        <v>160</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:Z3" si="49">C2+E2</f>
+        <v>110</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="49"/>
+        <v>110</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="49"/>
+        <v>250</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="49"/>
+        <v>160</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3" si="50">AA2+AC2</f>
+        <v>110</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3" si="51">AB2+AD2</f>
+        <v>250</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" ref="AC3" si="52">AC2+AE2</f>
+        <v>160</v>
+      </c>
+      <c r="AD3">
+        <f t="shared" ref="AD3" si="53">AD2+AF2</f>
+        <v>110</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" ref="AE3" si="54">AE2+AG2</f>
+        <v>250</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3" si="55">AF2+AH2</f>
+        <v>160</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" ref="AG3" si="56">AG2+AI2</f>
+        <v>110</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" ref="AH3" si="57">AH2+AJ2</f>
+        <v>250</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" ref="AI3" si="58">AI2+AK2</f>
+        <v>160</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" ref="AJ3" si="59">AJ2+AL2</f>
+        <v>110</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" ref="AK3" si="60">AK2+AM2</f>
+        <v>250</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" ref="AL3" si="61">AL2+AN2</f>
+        <v>160</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" ref="AM3" si="62">AM2+AO2</f>
+        <v>110</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3" si="63">AN2+AP2</f>
+        <v>150</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" ref="AO3" si="64">AO2+AQ2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f>D2-B2</f>
+        <v>140</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:AO4" si="65">E2-C2</f>
+        <v>-90</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" si="65"/>
+        <v>-50</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="65"/>
+        <v>140</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="65"/>
+        <v>-90</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="65"/>
+        <v>-150</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="65"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <f>D3</f>
+        <v>250</v>
+      </c>
+      <c r="C5">
+        <f>B3</f>
+        <v>160</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:AO5" si="66">C3</f>
+        <v>110</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="66"/>
+        <v>250</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="66"/>
+        <v>160</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="66"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <f>D4</f>
+        <v>-50</v>
+      </c>
+      <c r="C6">
+        <f>B4</f>
+        <v>140</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:AO6" si="67">C4</f>
+        <v>-90</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" si="67"/>
+        <v>-50</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="67"/>
+        <v>140</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="67"/>
+        <v>-90</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="67"/>
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <f>E7</f>
+        <v>-140</v>
+      </c>
+      <c r="C7">
+        <f>B4+B6</f>
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:AO7" si="68">C4+C6</f>
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="AK7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="68"/>
+        <v>-140</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="68"/>
+        <v>90</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="68"/>
+        <v>50</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="68"/>
+        <v>-240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <f>E8</f>
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <f>B7</f>
+        <v>-140</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:AO9" si="69">C7</f>
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AK8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AL8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <f>E9</f>
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <f>B8</f>
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AJ9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AK9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AL9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="69"/>
+        <v>50</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="69"/>
+        <v>-140</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="69"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <f>E10</f>
+        <v>-190</v>
+      </c>
+      <c r="C10">
+        <f>B9-B7</f>
+        <v>230</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:AO10" si="70">C9-C7</f>
+        <v>-40</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="AL10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="70"/>
+        <v>230</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="70"/>
+        <v>-40</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" si="70"/>
+        <v>-190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <f>E11</f>
+        <v>-40</v>
+      </c>
+      <c r="C11">
+        <f>B10</f>
+        <v>-190</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:AO12" si="71">C10</f>
+        <v>230</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="AJ11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="AK11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="AL11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41">
+      <c r="A12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <f>D7</f>
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <f>B7</f>
+        <v>-140</v>
+      </c>
+      <c r="E12">
+        <f>D11</f>
+        <v>230</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="71"/>
+        <v>-40</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="71"/>
+        <v>-190</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="71"/>
+        <v>230</v>
+      </c>
+      <c r="I12">
+        <f>H7</f>
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>